<commit_message>
allow string cell style
</commit_message>
<xml_diff>
--- a/tests/__snapshots__/table.xlsx
+++ b/tests/__snapshots__/table.xlsx
@@ -112,7 +112,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,7 +419,7 @@
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="20" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,36 +430,36 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="20" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="20" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:3" ht="20" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
set width and height for table
</commit_message>
<xml_diff>
--- a/tests/__snapshots__/table.xlsx
+++ b/tests/__snapshots__/table.xlsx
@@ -419,7 +419,7 @@
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20" customHeight="1">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20" customHeight="1">
+    <row r="2" spans="1:3" ht="100" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -441,7 +441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20" customHeight="1">
+    <row r="3" spans="1:3" ht="100" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -452,7 +452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1">
+    <row r="4" spans="1:3" ht="100" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Update Python version and add cell comment feature
</commit_message>
<xml_diff>
--- a/tests/__snapshots__/table.xlsx
+++ b/tests/__snapshots__/table.xlsx
@@ -576,7 +576,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="2">
-        <v>45205.61624725109</v>
+        <v>45875.80224571651</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="100" customHeight="1">
@@ -590,7 +590,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="2">
-        <v>45205.61624725114</v>
+        <v>45875.80224571656</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="100" customHeight="1">
@@ -604,7 +604,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="2">
-        <v>45205.61624725116</v>
+        <v>45875.80224571659</v>
       </c>
     </row>
   </sheetData>

</xml_diff>